<commit_message>
Add time column and 2006 follow-up data
</commit_message>
<xml_diff>
--- a/CognitiveImpairment/StudyDocuments/Schagen Domains.xlsx
+++ b/CognitiveImpairment/StudyDocuments/Schagen Domains.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="320">
   <si>
     <t>Test</t>
   </si>
@@ -1016,6 +1016,282 @@
   </si>
   <si>
     <t>HC (n=27)</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>49.0 (8.9)</t>
+  </si>
+  <si>
+    <t>49.7 (7.7)</t>
+  </si>
+  <si>
+    <t>47.8 (9.1)</t>
+  </si>
+  <si>
+    <t>44.8 (6.6)</t>
+  </si>
+  <si>
+    <t>59.0 (11.9)</t>
+  </si>
+  <si>
+    <t>57.2 (8.2)</t>
+  </si>
+  <si>
+    <t>58.7 (12.3)</t>
+  </si>
+  <si>
+    <t>62.6 (10.3)</t>
+  </si>
+  <si>
+    <t>28.0 (8.7)</t>
+  </si>
+  <si>
+    <t>28.2 (8.5)</t>
+  </si>
+  <si>
+    <t>30.8 (9.3)</t>
+  </si>
+  <si>
+    <t>28.6 (10.5)</t>
+  </si>
+  <si>
+    <t>559.1 (51.9)</t>
+  </si>
+  <si>
+    <t>571.9 (57.5)</t>
+  </si>
+  <si>
+    <t>570.1 (60.3)</t>
+  </si>
+  <si>
+    <t>551,0 (59.2)</t>
+  </si>
+  <si>
+    <t>563.5 (50.9)</t>
+  </si>
+  <si>
+    <t>581.0 (51.9)</t>
+  </si>
+  <si>
+    <t>575.7 (58.9)</t>
+  </si>
+  <si>
+    <t>558.9 (59.0)</t>
+  </si>
+  <si>
+    <t>594.0 (50.5)</t>
+  </si>
+  <si>
+    <t>609.5 (48.4)</t>
+  </si>
+  <si>
+    <t>601.9 (56.3)</t>
+  </si>
+  <si>
+    <t>580.4 (56.1)</t>
+  </si>
+  <si>
+    <t>104.6 (27.0)</t>
+  </si>
+  <si>
+    <t>107.4 (26.4)</t>
+  </si>
+  <si>
+    <t>91.2 (15.6)</t>
+  </si>
+  <si>
+    <t>66.8 (23.1)</t>
+  </si>
+  <si>
+    <t>60.1 (18.1)</t>
+  </si>
+  <si>
+    <t>73.7 (28.1)</t>
+  </si>
+  <si>
+    <t>62.1 (22.3)</t>
+  </si>
+  <si>
+    <t>113.6 (29.8)</t>
+  </si>
+  <si>
+    <t>113.6 (29.1)</t>
+  </si>
+  <si>
+    <t>106.1 (39.8)</t>
+  </si>
+  <si>
+    <t>112.2 (30.1)</t>
+  </si>
+  <si>
+    <t>58.4 (35.6)</t>
+  </si>
+  <si>
+    <t>55.6 (36.7)</t>
+  </si>
+  <si>
+    <t>62.5 (49.2)</t>
+  </si>
+  <si>
+    <t>61.1 (46.3)</t>
+  </si>
+  <si>
+    <t>11.2 (28.1)</t>
+  </si>
+  <si>
+    <t>5.1 (32.8)</t>
+  </si>
+  <si>
+    <t>14.1 (35.6)</t>
+  </si>
+  <si>
+    <t>12.8 (33.4)</t>
+  </si>
+  <si>
+    <t>616.4 (80.7)</t>
+  </si>
+  <si>
+    <t>650.7 (96.8)</t>
+  </si>
+  <si>
+    <t>651.4 (107.9)</t>
+  </si>
+  <si>
+    <t>599.9 (90.4)</t>
+  </si>
+  <si>
+    <t>59.2 (9.3)</t>
+  </si>
+  <si>
+    <t>57.2 (9.7)</t>
+  </si>
+  <si>
+    <t>57.8 (8.7)</t>
+  </si>
+  <si>
+    <t>59.9 (8.4)</t>
+  </si>
+  <si>
+    <t>13.8 ( 2.4)</t>
+  </si>
+  <si>
+    <t>13.6 ( 2.5)</t>
+  </si>
+  <si>
+    <t>13.2 (2.7)</t>
+  </si>
+  <si>
+    <t>14.1 (2.2)</t>
+  </si>
+  <si>
+    <t>15.6 (0.7)</t>
+  </si>
+  <si>
+    <t>15.5 ( 0.7)</t>
+  </si>
+  <si>
+    <t>15.2 (1.1)</t>
+  </si>
+  <si>
+    <t>15.5 (0.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.6 (4.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.8 (3.5) </t>
+  </si>
+  <si>
+    <t> 33.2 (4.7)</t>
+  </si>
+  <si>
+    <t>35.3 (3.6)</t>
+  </si>
+  <si>
+    <t>31.7 (6.2)</t>
+  </si>
+  <si>
+    <t>32.1 (5.6)</t>
+  </si>
+  <si>
+    <t>31.2 (5.7)</t>
+  </si>
+  <si>
+    <t>33.6 (4.6)</t>
+  </si>
+  <si>
+    <t>86.8 (11.5)</t>
+  </si>
+  <si>
+    <t>88.2 (9.6)</t>
+  </si>
+  <si>
+    <t>84.6 (12.3)</t>
+  </si>
+  <si>
+    <t>89.2 (11.1)</t>
+  </si>
+  <si>
+    <t>76.6 (11.8)</t>
+  </si>
+  <si>
+    <t>78.6 (10.5)</t>
+  </si>
+  <si>
+    <t>76.0 (13.5)</t>
+  </si>
+  <si>
+    <t>80.8 (11.5)</t>
+  </si>
+  <si>
+    <t>73.4 (12.1)</t>
+  </si>
+  <si>
+    <t>74.5 (13.2)</t>
+  </si>
+  <si>
+    <t>68.7 (13.8)</t>
+  </si>
+  <si>
+    <t>74.9 (10.3)</t>
+  </si>
+  <si>
+    <t>23.0 (5.6)</t>
+  </si>
+  <si>
+    <t>21.9 ( 4.6)</t>
+  </si>
+  <si>
+    <t>22.3 (4.8)</t>
+  </si>
+  <si>
+    <t>23.0 (5.0)</t>
+  </si>
+  <si>
+    <t>57.8 (7.5)</t>
+  </si>
+  <si>
+    <t>56.9 (7.7)</t>
+  </si>
+  <si>
+    <t>58.6 (7.8)</t>
+  </si>
+  <si>
+    <t>56.2 (6.7)</t>
+  </si>
+  <si>
+    <t>51.0 (6.4)</t>
+  </si>
+  <si>
+    <t>51.2 (9.5)</t>
+  </si>
+  <si>
+    <t>52.0 (8.3)</t>
+  </si>
+  <si>
+    <t>51.4 (7.3)</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1098,11 +1374,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1128,6 +1413,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1401,7 +1689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1409,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,14 +1708,14 @@
     <col min="1" max="1" width="28" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="5.140625" style="6" customWidth="1"/>
+    <col min="5" max="6" width="11.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -1437,20 +1725,23 @@
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1458,60 +1749,69 @@
         <v>37</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1521,120 +1821,138 @@
       <c r="C5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>4</v>
       </c>
@@ -1644,140 +1962,161 @@
       <c r="C11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
@@ -1787,20 +2126,23 @@
       <c r="C18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>6</v>
       </c>
@@ -1810,20 +2152,23 @@
       <c r="C19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>4</v>
       </c>
@@ -1833,120 +2178,705 @@
       <c r="C20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="6">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="F25" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="H25" s="10" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="6">
+        <v>12</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="6">
+        <v>12</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="6">
+        <v>12</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="6">
+        <v>12</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="6">
+        <v>12</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="6">
+        <v>12</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="6">
+        <v>12</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="6">
+        <v>12</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="6">
+        <v>12</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="6">
+        <v>12</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="6">
+        <v>12</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="6">
+        <v>12</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="6">
+        <v>12</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="6">
+        <v>12</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="6">
+        <v>12</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="6">
+        <v>12</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="6">
+        <v>12</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="6">
+        <v>12</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="6">
+        <v>12</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="6">
+        <v>12</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="6">
+        <v>12</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="6">
+        <v>12</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="6">
+        <v>12</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="6">
+        <v>12</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1955,24 +2885,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>221</v>
       </c>
@@ -1982,20 +2911,23 @@
       <c r="C1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2005,20 +2937,24 @@
       <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="2">
+        <f>11.5*12</f>
+        <v>138</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2028,20 +2964,24 @@
       <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D16" si="0">11.5*12</f>
+        <v>138</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -2051,20 +2991,24 @@
       <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2074,20 +3018,24 @@
       <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2097,20 +3045,24 @@
       <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2120,40 +3072,48 @@
       <c r="C7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2163,20 +3123,24 @@
       <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="H9" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2186,136 +3150,164 @@
       <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="H12" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="H14" s="11" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="H15" s="11" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>